<commit_message>
Committer: ANIORT Vincent INNOV/IT-S <SLRQ4050@orange.com> Final On branch main
</commit_message>
<xml_diff>
--- a/jour 2/Design_ergo_a11y/tests-CONCEPTEUR.xlsx
+++ b/jour 2/Design_ergo_a11y/tests-CONCEPTEUR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrq4050\Desktop\test_ergo_a11y\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrq4050\Documents\vince\master2ergo\2022\jour 2\Design_ergo_a11y\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B164D908-1179-460B-8CEE-DBF2FE405B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DAE419-97C9-40CF-9A80-3EFA5E9AA35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="24645" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tests" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="59">
   <si>
     <t>Contenu textuel</t>
   </si>
@@ -291,17 +291,6 @@
     Les éléments en mouvement perturbent certains utilisateurs et rendent difficile la lecture (notamment les personnes malvoyantes, épileptiques, ou ayant des problèmes d’attention). Ils doivent donc par défaut être en pause au chargement de la page
     Si des animations sont en lecture automatique, il est primordial de pouvoir les arrêter ou les cacher
     Les flashs lumineux ou tout élément clignotant ont un fort impact sur les utilisateurs épileptiques, et vont également perturber l’attention de tous les utilisateurs
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Procédures
-    Examiner les wireframes et les maquettes graphiques
-    Examiner les parcours utilisateurs et les spécifications associées
-A vérifier
-    Quel que soit le parcours, seules les actions demandées par l’utilisateur sont exécutées et l’utilisateur peut toujours les interrompre. L'utilisateur contrôle le système
-Justification
-    L’utilisateur doit contrôler le système et non l’inverse.
-    C’est encore plus important, si l’utilisateur ne voit pas ce qu’il se passe à l’écran, il peut vite être perdu, si le système prend la main sans l’en avertir. Ainsi, la validation d'un formulaire ne doit pas être automatique mais nécessiter une activation explicite d'un bouton par l'utilisateur. De la même façon, la mise à jour d'une application ou le téléchargement d'un nouvel élément doit se faire avec l'accord de l'utilisateur
 </t>
   </si>
   <si>
@@ -1212,7 +1201,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau15" displayName="Tableau15" ref="A2:B31" headerRowCount="0" totalsRowShown="0" headerRowBorderDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau15" displayName="Tableau15" ref="A2:B30" headerRowCount="0" totalsRowShown="0" headerRowBorderDxfId="39" tableBorderDxfId="38">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" headerRowDxfId="37" dataDxfId="36" totalsRowDxfId="35"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Colonne3" headerRowDxfId="34" dataDxfId="33"/>
@@ -1575,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B187"/>
+  <dimension ref="A1:B186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,133 +1676,129 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="192.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="228" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="228" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="16" t="s">
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="15"/>
+    </row>
+    <row r="18" spans="1:2" ht="228" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:2" ht="228" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="204" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="204" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="216.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="216.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="17" t="s">
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:2" ht="324" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="15"/>
-    </row>
-    <row r="23" spans="1:2" ht="324" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="16" t="s">
+    <row r="23" spans="1:2" ht="252.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="252.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="240.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="240.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="17" t="s">
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="18"/>
+    </row>
+    <row r="26" spans="1:2" ht="312.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="18"/>
-    </row>
-    <row r="27" spans="1:2" ht="312.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="17" t="s">
+    <row r="28" spans="1:2" ht="36" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="18"/>
+    </row>
+    <row r="29" spans="1:2" ht="156.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="36" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="18"/>
-    </row>
-    <row r="30" spans="1:2" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="180.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>58</v>
-      </c>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="20"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
@@ -2434,10 +2419,6 @@
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="5"/>
       <c r="B186" s="20"/>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="5"/>
-      <c r="B187" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>